<commit_message>
found out sample with bag
</commit_message>
<xml_diff>
--- a/TestExampleResults.xlsx
+++ b/TestExampleResults.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anvarshagvaleev/Education/DataScience/University/Graduate/MasterWork/BestMetric/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{512F9BD9-F097-144D-A93F-5C5D02A87B4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6184F8D-1B80-D047-B908-82DD48DBC3B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" activeTab="1" xr2:uid="{37B94DBA-A1EA-3348-9ABB-58D18268F39D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15980" xr2:uid="{37B94DBA-A1EA-3348-9ABB-58D18268F39D}"/>
   </bookViews>
   <sheets>
     <sheet name="MinMax" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="16">
   <si>
     <t>(1,2)</t>
   </si>
@@ -64,6 +64,24 @@
   </si>
   <si>
     <t>(0, 3)</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>(3,4)</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>(0,2)</t>
+  </si>
+  <si>
+    <t>((0,2), 1)</t>
+  </si>
+  <si>
+    <t>(((0,2), 1), (3,4))</t>
   </si>
 </sst>
 </file>
@@ -106,7 +124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -119,9 +137,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -437,15 +452,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3949D843-A64C-0840-AFDD-CED77C4DF9BE}">
-  <dimension ref="B2:F25"/>
+  <dimension ref="B2:N29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="6" width="15.6640625" customWidth="1"/>
+    <col min="7" max="7" width="7" customWidth="1"/>
+    <col min="8" max="8" width="7.5" customWidth="1"/>
+    <col min="9" max="14" width="15.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C2" s="2">
         <v>0</v>
       </c>
@@ -458,8 +479,23 @@
       <c r="F2" s="2">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="J2" s="2">
+        <v>0</v>
+      </c>
+      <c r="K2" s="3">
+        <v>1</v>
+      </c>
+      <c r="L2" s="3">
+        <v>2</v>
+      </c>
+      <c r="M2" s="2">
+        <v>3</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B3" s="4">
         <v>0</v>
       </c>
@@ -475,8 +511,26 @@
       <c r="F3" s="1">
         <v>0.60917100000000002</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="I3" s="4">
+        <v>0</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0</v>
+      </c>
+      <c r="K3" s="1">
+        <v>50.319479000000001</v>
+      </c>
+      <c r="L3" s="1">
+        <v>23.586649000000001</v>
+      </c>
+      <c r="M3" s="1">
+        <v>96.871926000000002</v>
+      </c>
+      <c r="N3" s="1">
+        <v>75.555873000000005</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B4" s="4">
         <v>1</v>
       </c>
@@ -492,8 +546,26 @@
       <c r="F4" s="1">
         <v>1.4429149999999999</v>
       </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="I4" s="4">
+        <v>1</v>
+      </c>
+      <c r="J4" s="1">
+        <v>50.319479000000001</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0</v>
+      </c>
+      <c r="L4" s="1">
+        <v>73.279329000000004</v>
+      </c>
+      <c r="M4" s="1">
+        <v>145.971847</v>
+      </c>
+      <c r="N4">
+        <v>125.45222200000001</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B5" s="4">
         <v>2</v>
       </c>
@@ -509,8 +581,26 @@
       <c r="F5" s="1">
         <v>1.274184</v>
       </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="I5" s="4">
+        <v>2</v>
+      </c>
+      <c r="J5" s="1">
+        <v>23.586649000000001</v>
+      </c>
+      <c r="K5" s="1">
+        <v>73.279329000000004</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0</v>
+      </c>
+      <c r="M5" s="1">
+        <v>73.286287999999999</v>
+      </c>
+      <c r="N5">
+        <v>52.184671999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B6" s="4">
         <v>3</v>
       </c>
@@ -526,8 +616,46 @@
       <c r="F6" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="I6" s="4">
+        <v>3</v>
+      </c>
+      <c r="J6" s="1">
+        <v>96.871926000000002</v>
+      </c>
+      <c r="K6" s="1">
+        <v>145.971847</v>
+      </c>
+      <c r="L6" s="1">
+        <v>73.286287999999999</v>
+      </c>
+      <c r="M6" s="1">
+        <v>0</v>
+      </c>
+      <c r="N6">
+        <v>23.104112000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="I7" s="4">
+        <v>4</v>
+      </c>
+      <c r="J7" s="1">
+        <v>75.555873000000005</v>
+      </c>
+      <c r="K7">
+        <v>125.45222200000001</v>
+      </c>
+      <c r="L7">
+        <v>52.184671999999999</v>
+      </c>
+      <c r="M7">
+        <v>23.104112000000001</v>
+      </c>
+      <c r="N7" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
       <c r="C10" s="2" t="s">
         <v>0</v>
       </c>
@@ -537,8 +665,20 @@
       <c r="E10" s="3">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="J10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0</v>
+      </c>
+      <c r="L10" s="3">
+        <v>1</v>
+      </c>
+      <c r="M10" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B11" s="4" t="s">
         <v>0</v>
       </c>
@@ -553,8 +693,26 @@
         <f>(D6+E6)/2</f>
         <v>1.3585495000000001</v>
       </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="I11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="1">
+        <f>(M3+N3)/2</f>
+        <v>86.213899499999997</v>
+      </c>
+      <c r="L11" s="1">
+        <f>(M4+N4)/2</f>
+        <v>135.71203450000002</v>
+      </c>
+      <c r="M11" s="1">
+        <f>(M5+N5)/2</f>
+        <v>62.735479999999995</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B12" s="4">
         <v>0</v>
       </c>
@@ -569,8 +727,26 @@
         <f>F3</f>
         <v>0.60917100000000002</v>
       </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="I12" s="4">
+        <v>0</v>
+      </c>
+      <c r="J12" s="1">
+        <f>K11</f>
+        <v>86.213899499999997</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0</v>
+      </c>
+      <c r="L12" s="1">
+        <f>K3</f>
+        <v>50.319479000000001</v>
+      </c>
+      <c r="M12" s="1">
+        <f>L3</f>
+        <v>23.586649000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B13" s="4">
         <v>3</v>
       </c>
@@ -585,16 +761,63 @@
       <c r="E13" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="I13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="J13" s="1">
+        <f>L11</f>
+        <v>135.71203450000002</v>
+      </c>
+      <c r="K13" s="1">
+        <f>L12</f>
+        <v>50.319479000000001</v>
+      </c>
+      <c r="L13" s="1">
+        <v>0</v>
+      </c>
+      <c r="M13" s="1">
+        <f>L4</f>
+        <v>73.279329000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="I14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="J14" s="1">
+        <f>M11</f>
+        <v>62.735479999999995</v>
+      </c>
+      <c r="K14" s="1">
+        <f>M12</f>
+        <v>23.586649000000001</v>
+      </c>
+      <c r="L14" s="1">
+        <f>M13</f>
+        <v>73.279329000000004</v>
+      </c>
+      <c r="M14" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C17" s="2" t="s">
         <v>1</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="J17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L17" s="3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
         <v>1</v>
       </c>
@@ -605,8 +828,22 @@
         <f>(E3+D6)/2</f>
         <v>1.0630519999999999</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="I18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0</v>
+      </c>
+      <c r="K18" s="1">
+        <f>(MIN(M3,N3,M5,N5)+MAX(M3,N3,M5,N5))/2</f>
+        <v>74.528299000000004</v>
+      </c>
+      <c r="L18">
+        <f>(J4+L4)/2</f>
+        <v>61.799404000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
         <v>0</v>
       </c>
@@ -617,13 +854,52 @@
       <c r="D19" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="I19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J19" s="1">
+        <f>K18</f>
+        <v>74.528299000000004</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <f>(M4+N4)/2</f>
+        <v>135.71203450000002</v>
+      </c>
+    </row>
+    <row r="20" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="I20" s="3">
+        <v>1</v>
+      </c>
+      <c r="J20">
+        <f>L18</f>
+        <v>61.799404000000003</v>
+      </c>
+      <c r="K20">
+        <f>L19</f>
+        <v>135.71203450000002</v>
+      </c>
+      <c r="L20" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="L21" s="1"/>
+    </row>
+    <row r="23" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C23" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="J23" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
         <v>7</v>
       </c>
@@ -631,10 +907,43 @@
         <v>0</v>
       </c>
       <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="I24" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J24" s="1">
+        <v>0</v>
+      </c>
+      <c r="K24" s="1">
+        <f>(MIN(M3,N3,M4,N4,M5,N5)+ MAX(M3,N3,M4,N4,M5,N5))/2</f>
+        <v>99.078259500000001</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" x14ac:dyDescent="0.2">
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
+      <c r="I25" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J25" s="1">
+        <f>K24</f>
+        <v>99.078259500000001</v>
+      </c>
+      <c r="K25" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="J28" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="I29" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="J29" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -648,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B974118E-A2A7-E442-812E-EB01D78CF4BF}">
   <dimension ref="B2:N24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -821,10 +1130,10 @@
       <c r="K10" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L10" s="5">
-        <v>0</v>
-      </c>
-      <c r="M10" s="5">
+      <c r="L10" s="3">
+        <v>0</v>
+      </c>
+      <c r="M10" s="3">
         <v>3</v>
       </c>
     </row>
@@ -873,7 +1182,7 @@
         <f>F5</f>
         <v>5.0990195099999998</v>
       </c>
-      <c r="J12" s="5">
+      <c r="J12" s="3">
         <v>0</v>
       </c>
       <c r="K12" s="1">
@@ -903,7 +1212,7 @@
       <c r="E13" s="1">
         <v>0</v>
       </c>
-      <c r="J13" s="5">
+      <c r="J13" s="3">
         <v>3</v>
       </c>
       <c r="K13" s="1">

</xml_diff>